<commit_message>
Home page UI tests done
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA6AC29-4F34-4FE1-9564-0165E8F4CFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC5D285-5E42-4E5E-A944-6D1FA8225B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
   <si>
     <t>Test plan</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Home Screen</t>
   </si>
   <si>
-    <t>H-001 Correctness of URL and title</t>
-  </si>
-  <si>
     <t>Check if the URL and title contain correct data</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>Browser successfully launched</t>
   </si>
   <si>
-    <t>Check upper grid images effect on hover</t>
-  </si>
-  <si>
     <t>Move mouse to each of the images in upper grid</t>
   </si>
   <si>
@@ -155,19 +149,7 @@
     <t>Check that images get bigger on hover</t>
   </si>
   <si>
-    <t>H-004 Upper marquee products count</t>
-  </si>
-  <si>
-    <t>Check if upper marquee contains 3 products</t>
-  </si>
-  <si>
-    <t>Check that upper marquee contains 3 products</t>
-  </si>
-  <si>
     <t>Scroll down to see the marquee</t>
-  </si>
-  <si>
-    <t>H-005 Shopify information header and content</t>
   </si>
   <si>
     <t>Check if shopify info part contains correct header and content</t>
@@ -177,12 +159,6 @@
   </si>
   <si>
     <t>Check that it contains correct header and content</t>
-  </si>
-  <si>
-    <t>H-006 Shopify information link redirect</t>
-  </si>
-  <si>
-    <t>Check if link in Shopify information part is redirecting correctly</t>
   </si>
   <si>
     <r>
@@ -213,62 +189,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">Check if user is redirected to </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>shopify.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Check if lower grid contains 3 products</t>
-  </si>
-  <si>
     <t>Scroll down to lower product grid</t>
   </si>
   <si>
     <t>Check that lower grid contains 3 products</t>
-  </si>
-  <si>
-    <t>H-007 Lower grid products count</t>
-  </si>
-  <si>
-    <t>H-008 Lower grid images effect</t>
-  </si>
-  <si>
-    <t>Move mouse to each of the images in lower grid</t>
-  </si>
-  <si>
-    <t>H-009 Lower marquee products count</t>
-  </si>
-  <si>
-    <t>Check if lower marquee contains 1 product</t>
-  </si>
-  <si>
-    <t>Scroll down to see the lower marquee</t>
-  </si>
-  <si>
-    <t>Check that lower marquee contains 1 product</t>
-  </si>
-  <si>
-    <t>H-010 Link redirection in footer</t>
   </si>
   <si>
     <t>Check links in footer redirect user to correct pages</t>
@@ -302,23 +226,6 @@
         <scheme val="major"/>
       </rPr>
       <t xml:space="preserve"> button</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Check if user is correctly redirected to </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>shopify.com</t>
     </r>
   </si>
   <si>
@@ -370,9 +277,6 @@
     </r>
   </si>
   <si>
-    <t>H-011 Change website background</t>
-  </si>
-  <si>
     <t>Check if background changing function is working correctly</t>
   </si>
   <si>
@@ -405,9 +309,6 @@
     <t>Change website background to Dark</t>
   </si>
   <si>
-    <t>H-012 Change website language</t>
-  </si>
-  <si>
     <t>Check if is possible to change the language of website</t>
   </si>
   <si>
@@ -420,22 +321,107 @@
     <t>Change website language to English</t>
   </si>
   <si>
-    <t>H-013 Change website language</t>
-  </si>
-  <si>
-    <t>Check if link in GitHub logo is working properly</t>
-  </si>
-  <si>
     <t>Click on GitHub logo</t>
   </si>
   <si>
     <t>Check if user is redirected to Vercel GitHub</t>
   </si>
   <si>
-    <t>Check if upper grid contains 3 products and check image hover effect</t>
+    <t>H-003 Sliders products count</t>
   </si>
   <si>
-    <t>H-002 Upper grid products</t>
+    <t>Check if upper slider contains 3 products and lower slider 1 product</t>
+  </si>
+  <si>
+    <t>Check that upper slider contains 3 products</t>
+  </si>
+  <si>
+    <t>Scroll down to see the lower slider</t>
+  </si>
+  <si>
+    <t>Check that lower slider contains 1 product</t>
+  </si>
+  <si>
+    <t>H-004 Shopify information header and content</t>
+  </si>
+  <si>
+    <t>H-006 Change website background</t>
+  </si>
+  <si>
+    <t>H-007 Change website language</t>
+  </si>
+  <si>
+    <t>Check if each of the grids contain 3 products and check image hover effect</t>
+  </si>
+  <si>
+    <t>Upper grid contains 3 products</t>
+  </si>
+  <si>
+    <t>Hover effect is working properly</t>
+  </si>
+  <si>
+    <t>Lower product grid is visible</t>
+  </si>
+  <si>
+    <t>Each of the images is visible</t>
+  </si>
+  <si>
+    <t>Lower grid contains 3 products</t>
+  </si>
+  <si>
+    <t>H-002 Grid products count and effect</t>
+  </si>
+  <si>
+    <t>H-001 Correctness of URL and title and cookies acceptance</t>
+  </si>
+  <si>
+    <t>Check if cookies banner is not visible</t>
+  </si>
+  <si>
+    <t>Cookies banner is not visible (cookies are accepted before each test case)</t>
+  </si>
+  <si>
+    <t>Check that upper slider contains: Train&amp;Sleep T-shirt, Nike T-shirt, QR code</t>
+  </si>
+  <si>
+    <t>Check that lower slider contains: Code Shirt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check if user is redirected to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>shopify.vercel.store</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check if user is correctly redirected to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>shopify.vercel.store</t>
+    </r>
+  </si>
+  <si>
+    <t>H-005 Link redirections in footer</t>
   </si>
 </sst>
 </file>
@@ -555,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -579,6 +565,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -599,16 +592,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1014,162 +997,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
-  <dimension ref="A1:V885"/>
+  <dimension ref="A1:V873"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="13">
+      <c r="B5" s="18"/>
+      <c r="C5" s="16">
         <f ca="1">TODAY()</f>
-        <v>44979</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
+        <v>44980</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
     </row>
     <row r="7" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -1198,22 +1181,22 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
@@ -1222,16 +1205,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
@@ -1241,16 +1224,16 @@
         <v>2</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -1260,545 +1243,615 @@
         <v>3</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7">
+        <v>4</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B13" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7">
-        <v>1</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="C13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="7">
+        <v>4</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="7">
         <v>5</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="6">
-        <v>4</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="E18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+        <v>57</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="7">
         <v>1</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F24" s="2"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="7">
         <v>2</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="7">
         <v>3</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>40</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="7">
         <v>4</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>41</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="7">
+        <v>5</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="7">
+        <v>6</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="7">
+        <v>7</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="7">
+        <v>8</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B32" s="6">
+        <v>4</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D34" s="7">
+        <v>2</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D35" s="7">
+        <v>3</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D36" s="7">
+        <v>4</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D37" s="7">
+        <v>5</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D38" s="7">
         <v>6</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="7">
-        <v>1</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D30" s="7">
-        <v>2</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D31" s="7">
-        <v>3</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D32" s="7">
-        <v>4</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D33" s="19">
+      <c r="E38" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="6">
         <v>5</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="6">
-        <v>7</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="18"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="7">
-        <v>1</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="7">
-        <v>2</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="19">
-        <v>3</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="7">
-        <v>4</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="6">
-        <v>8</v>
-      </c>
       <c r="C39" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+        <v>79</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="7">
         <v>1</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="7">
         <v>2</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="19">
+      <c r="D42" s="7">
         <v>3</v>
       </c>
-      <c r="E42" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="2"/>
+      <c r="E42" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="7">
         <v>4</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F43" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="7">
+      <c r="D44" s="2">
         <v>5</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F44" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" s="6">
-        <v>9</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F45" s="18"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="2">
+        <v>6</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="7">
-        <v>1</v>
+      <c r="D46" s="2">
+        <v>7</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="F46" s="8"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="7">
-        <v>2</v>
+      <c r="D47" s="2">
+        <v>8</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F47" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="7">
-        <v>3</v>
+      <c r="D48" s="2">
+        <v>9</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F48" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="7">
-        <v>4</v>
+      <c r="D49" s="2">
+        <v>10</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="2">
+        <v>11</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="6">
-        <v>10</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F50" s="18"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="7">
-        <v>1</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
+      <c r="B51" s="6">
+        <v>6</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="11"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
@@ -1809,10 +1862,10 @@
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
@@ -1823,10 +1876,10 @@
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
@@ -1836,11 +1889,11 @@
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="2">
-        <v>5</v>
+      <c r="D55" s="7">
+        <v>4</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
@@ -1851,10 +1904,10 @@
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="D56" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
@@ -1865,10 +1918,10 @@
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="D57" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
@@ -1879,70 +1932,70 @@
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" s="6">
-        <v>11</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" s="18"/>
-      <c r="E59" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="F59" s="18"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="2">
+        <v>8</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="7">
-        <v>1</v>
+      <c r="D60" s="2">
+        <v>9</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="7">
-        <v>2</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
+      <c r="A61" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" s="6">
+        <v>7</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D61" s="11"/>
+      <c r="E61" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" s="11"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="D62" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
@@ -1953,10 +2006,10 @@
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
@@ -1966,11 +2019,11 @@
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="2">
-        <v>5</v>
+      <c r="D64" s="7">
+        <v>3</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
@@ -1980,11 +2033,11 @@
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="2">
-        <v>6</v>
+      <c r="D65" s="7">
+        <v>4</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
@@ -1995,10 +2048,10 @@
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
@@ -2009,10 +2062,10 @@
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
@@ -2023,43 +2076,27 @@
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
       <c r="D68" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B69" s="6">
-        <v>12</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D69" s="18"/>
-      <c r="E69" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F69" s="18"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="7">
-        <v>1</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
@@ -2068,12 +2105,8 @@
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="7">
-        <v>2</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
@@ -2082,12 +2115,8 @@
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="7">
-        <v>3</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
@@ -2096,12 +2125,8 @@
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="7">
-        <v>4</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>73</v>
-      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
@@ -2110,12 +2135,8 @@
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="2">
-        <v>5</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>74</v>
-      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -2124,12 +2145,8 @@
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="2">
-        <v>6</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>75</v>
-      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
@@ -2138,44 +2155,28 @@
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="2">
-        <v>7</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>74</v>
-      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A77" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B77" s="6">
-        <v>13</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D77" s="18"/>
-      <c r="E77" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F77" s="18"/>
-      <c r="G77" s="16"/>
-      <c r="H77" s="16"/>
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="7">
-        <v>1</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="8"/>
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
@@ -2184,12 +2185,8 @@
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="7">
-        <v>2</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="8"/>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
@@ -2198,12 +2195,8 @@
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="7">
-        <v>3</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="8"/>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
@@ -2212,12 +2205,8 @@
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="7">
-        <v>4</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>78</v>
-      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="8"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -2226,12 +2215,8 @@
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
-      <c r="D82" s="2">
-        <v>5</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="8"/>
       <c r="F82" s="8"/>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
@@ -10145,126 +10130,6 @@
       <c r="F873" s="8"/>
       <c r="G873" s="8"/>
       <c r="H873" s="8"/>
-    </row>
-    <row r="874" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A874" s="8"/>
-      <c r="B874" s="8"/>
-      <c r="C874" s="8"/>
-      <c r="D874" s="2"/>
-      <c r="E874" s="8"/>
-      <c r="F874" s="8"/>
-      <c r="G874" s="8"/>
-      <c r="H874" s="8"/>
-    </row>
-    <row r="875" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A875" s="8"/>
-      <c r="B875" s="8"/>
-      <c r="C875" s="8"/>
-      <c r="D875" s="2"/>
-      <c r="E875" s="8"/>
-      <c r="F875" s="8"/>
-      <c r="G875" s="8"/>
-      <c r="H875" s="8"/>
-    </row>
-    <row r="876" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A876" s="8"/>
-      <c r="B876" s="8"/>
-      <c r="C876" s="8"/>
-      <c r="D876" s="2"/>
-      <c r="E876" s="8"/>
-      <c r="F876" s="8"/>
-      <c r="G876" s="8"/>
-      <c r="H876" s="8"/>
-    </row>
-    <row r="877" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A877" s="8"/>
-      <c r="B877" s="8"/>
-      <c r="C877" s="8"/>
-      <c r="D877" s="2"/>
-      <c r="E877" s="8"/>
-      <c r="F877" s="8"/>
-      <c r="G877" s="8"/>
-      <c r="H877" s="8"/>
-    </row>
-    <row r="878" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A878" s="8"/>
-      <c r="B878" s="8"/>
-      <c r="C878" s="8"/>
-      <c r="D878" s="2"/>
-      <c r="E878" s="8"/>
-      <c r="F878" s="8"/>
-      <c r="G878" s="8"/>
-      <c r="H878" s="8"/>
-    </row>
-    <row r="879" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A879" s="8"/>
-      <c r="B879" s="8"/>
-      <c r="C879" s="8"/>
-      <c r="D879" s="2"/>
-      <c r="E879" s="8"/>
-      <c r="F879" s="8"/>
-      <c r="G879" s="8"/>
-      <c r="H879" s="8"/>
-    </row>
-    <row r="880" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A880" s="8"/>
-      <c r="B880" s="8"/>
-      <c r="C880" s="8"/>
-      <c r="D880" s="2"/>
-      <c r="E880" s="8"/>
-      <c r="F880" s="8"/>
-      <c r="G880" s="8"/>
-      <c r="H880" s="8"/>
-    </row>
-    <row r="881" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A881" s="8"/>
-      <c r="B881" s="8"/>
-      <c r="C881" s="8"/>
-      <c r="D881" s="2"/>
-      <c r="E881" s="8"/>
-      <c r="F881" s="8"/>
-      <c r="G881" s="8"/>
-      <c r="H881" s="8"/>
-    </row>
-    <row r="882" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A882" s="8"/>
-      <c r="B882" s="8"/>
-      <c r="C882" s="8"/>
-      <c r="D882" s="2"/>
-      <c r="E882" s="8"/>
-      <c r="F882" s="8"/>
-      <c r="G882" s="8"/>
-      <c r="H882" s="8"/>
-    </row>
-    <row r="883" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A883" s="8"/>
-      <c r="B883" s="8"/>
-      <c r="C883" s="8"/>
-      <c r="D883" s="2"/>
-      <c r="E883" s="8"/>
-      <c r="F883" s="8"/>
-      <c r="G883" s="8"/>
-      <c r="H883" s="8"/>
-    </row>
-    <row r="884" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A884" s="8"/>
-      <c r="B884" s="8"/>
-      <c r="C884" s="8"/>
-      <c r="D884" s="2"/>
-      <c r="E884" s="8"/>
-      <c r="F884" s="8"/>
-      <c r="G884" s="8"/>
-      <c r="H884" s="8"/>
-    </row>
-    <row r="885" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A885" s="8"/>
-      <c r="B885" s="8"/>
-      <c r="C885" s="8"/>
-      <c r="D885" s="2"/>
-      <c r="E885" s="8"/>
-      <c r="F885" s="8"/>
-      <c r="G885" s="8"/>
-      <c r="H885" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -10278,7 +10143,7 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F9:F11 F19:F22 F24:F27 F29:F33 F35:F38 F40:F44 F46:F49 F51:F58 F60:F68 F70:F76 F78:F100 F13:F17">
+  <conditionalFormatting sqref="F33:F38 F40:F50 F52:F60 F14:F22 F9:F12 F24:F31 F62:F88">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F9="Open"</formula>
     </cfRule>
@@ -10304,7 +10169,7 @@
           <x14:formula1>
             <xm:f>'Possible results'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F9:F11 F35:F37 F40:F43 F13:F16</xm:sqref>
+          <xm:sqref>F14:F22 F9:F12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Home UX test in progress
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC5D285-5E42-4E5E-A944-6D1FA8225B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A005916-451F-47EF-B690-E3F750E8EB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
   <si>
     <t>Test plan</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>https://learn.cypress.io/tutorials/creating-a-shopify-partners-store</t>
-  </si>
-  <si>
-    <t>Home Screen</t>
   </si>
   <si>
     <t>Check if the URL and title contain correct data</t>
@@ -423,12 +420,135 @@
   <si>
     <t>H-005 Link redirections in footer</t>
   </si>
+  <si>
+    <t>Home Screen UI</t>
+  </si>
+  <si>
+    <t>Home Screen UX</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>button in header</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Show all products by clicking on button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>All</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> and order them by different options</t>
+    </r>
+  </si>
+  <si>
+    <t>In option Price: Low to high check that prices are in ascending order</t>
+  </si>
+  <si>
+    <t>In option Price: High to low check that prices are in descending order</t>
+  </si>
+  <si>
+    <t>H-008 Show all products and order them</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">Home page </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>button in header</t>
+    </r>
+  </si>
+  <si>
+    <t>Check that page contains 2 products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that page contains 4 products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that page contains just products from list </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check that URL contains word </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>search</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,6 +616,14 @@
       <charset val="238"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -541,7 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,7 +721,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -997,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
-  <dimension ref="A1:V873"/>
+  <dimension ref="A1:V875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,7 +1259,7 @@
       <c r="B5" s="18"/>
       <c r="C5" s="16">
         <f ca="1">TODAY()</f>
-        <v>44980</v>
+        <v>44981</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -1182,17 +1309,17 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="9"/>
@@ -1205,16 +1332,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
@@ -1224,16 +1351,16 @@
         <v>2</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -1243,16 +1370,16 @@
         <v>3</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
@@ -1261,32 +1388,32 @@
       <c r="D12" s="7">
         <v>4</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>73</v>
+      <c r="E12" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="19" t="s">
-        <v>74</v>
+      <c r="G12" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B13" s="6">
         <v>2</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="9"/>
@@ -1299,16 +1426,16 @@
         <v>1</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
@@ -1318,16 +1445,16 @@
         <v>2</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -1337,16 +1464,16 @@
         <v>3</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1356,16 +1483,16 @@
         <v>4</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1375,16 +1502,16 @@
         <v>5</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1394,16 +1521,16 @@
         <v>6</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1413,16 +1540,16 @@
         <v>7</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1432,16 +1559,16 @@
         <v>8</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1451,31 +1578,31 @@
         <v>9</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B23" s="6">
         <v>3</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="9"/>
@@ -1488,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="8"/>
@@ -1501,7 +1628,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="8"/>
@@ -1514,7 +1641,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="8"/>
@@ -1527,7 +1654,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="8"/>
@@ -1539,8 +1666,8 @@
       <c r="D28" s="7">
         <v>5</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>75</v>
+      <c r="E28" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="8"/>
@@ -1553,7 +1680,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="8"/>
@@ -1566,7 +1693,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="8"/>
@@ -1579,7 +1706,7 @@
         <v>8</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="8"/>
@@ -1587,17 +1714,17 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B32" s="6">
         <v>4</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="9"/>
@@ -1608,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -1618,7 +1745,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1626,7 +1753,7 @@
         <v>3</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1634,7 +1761,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1642,7 +1769,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1650,22 +1777,22 @@
         <v>6</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B39" s="6">
         <v>5</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="9"/>
@@ -1679,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -1693,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
@@ -1707,7 +1834,7 @@
         <v>3</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
@@ -1721,7 +1848,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
@@ -1735,7 +1862,7 @@
         <v>5</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
@@ -1749,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -1763,7 +1890,7 @@
         <v>7</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -1777,7 +1904,7 @@
         <v>8</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -1791,7 +1918,7 @@
         <v>9</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
@@ -1805,7 +1932,7 @@
         <v>10</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
@@ -1819,7 +1946,7 @@
         <v>11</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
@@ -1827,17 +1954,17 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B51" s="6">
         <v>6</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="9"/>
@@ -1851,7 +1978,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
@@ -1865,7 +1992,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
@@ -1879,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
@@ -1893,7 +2020,7 @@
         <v>4</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
@@ -1907,7 +2034,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
@@ -1921,7 +2048,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
@@ -1935,7 +2062,7 @@
         <v>7</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
@@ -1949,7 +2076,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
@@ -1963,7 +2090,7 @@
         <v>9</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
@@ -1971,17 +2098,17 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B61" s="6">
         <v>7</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D61" s="11"/>
       <c r="E61" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F61" s="11"/>
       <c r="G61" s="9"/>
@@ -1995,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
@@ -2009,7 +2136,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
@@ -2023,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
@@ -2037,7 +2164,7 @@
         <v>4</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
@@ -2051,7 +2178,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
@@ -2065,7 +2192,7 @@
         <v>6</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
@@ -2079,24 +2206,40 @@
         <v>7</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
+      <c r="A69" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="6">
+        <v>8</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D69" s="11"/>
+      <c r="E69" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F69" s="11"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
+      <c r="D70" s="7">
+        <v>1</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
@@ -2105,8 +2248,12 @@
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="8"/>
+      <c r="D71" s="7">
+        <v>2</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
@@ -2115,8 +2262,12 @@
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="8"/>
+      <c r="D72" s="7">
+        <v>3</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>90</v>
+      </c>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
@@ -2125,8 +2276,12 @@
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="8"/>
+      <c r="D73" s="7">
+        <v>4</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
@@ -2135,8 +2290,12 @@
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="8"/>
+      <c r="D74" s="7">
+        <v>5</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -2145,8 +2304,12 @@
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="8"/>
+      <c r="D75" s="7">
+        <v>6</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
@@ -2155,8 +2318,12 @@
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="8"/>
+      <c r="D76" s="7">
+        <v>7</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
@@ -2165,8 +2332,12 @@
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="8"/>
+      <c r="D77" s="7">
+        <v>8</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="F77" s="8"/>
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
@@ -2175,8 +2346,12 @@
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="8"/>
+      <c r="D78" s="7">
+        <v>9</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
@@ -2185,8 +2360,12 @@
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="8"/>
+      <c r="D79" s="7">
+        <v>10</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
@@ -10130,6 +10309,26 @@
       <c r="F873" s="8"/>
       <c r="G873" s="8"/>
       <c r="H873" s="8"/>
+    </row>
+    <row r="874" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A874" s="8"/>
+      <c r="B874" s="8"/>
+      <c r="C874" s="8"/>
+      <c r="D874" s="2"/>
+      <c r="E874" s="8"/>
+      <c r="F874" s="8"/>
+      <c r="G874" s="8"/>
+      <c r="H874" s="8"/>
+    </row>
+    <row r="875" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A875" s="8"/>
+      <c r="B875" s="8"/>
+      <c r="C875" s="8"/>
+      <c r="D875" s="2"/>
+      <c r="E875" s="8"/>
+      <c r="F875" s="8"/>
+      <c r="G875" s="8"/>
+      <c r="H875" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -10143,7 +10342,7 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F33:F38 F40:F50 F52:F60 F14:F22 F9:F12 F24:F31 F62:F88">
+  <conditionalFormatting sqref="F33:F38 F40:F50 F52:F60 F14:F22 F9:F12 F24:F31 F62:F68 F70:F90">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F9="Open"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Home page test suite done
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA72AE6-D4D0-48EC-98E9-7B476D85F515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C07CB51-F5C7-40BA-8FBC-07A928F531F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="134">
   <si>
     <t>Test plan</t>
   </si>
@@ -708,9 +708,6 @@
   </si>
   <si>
     <t>Login testy</t>
-  </si>
-  <si>
-    <t>Registracia testy</t>
   </si>
   <si>
     <t>Prihlaseny uzivatel menu testy</t>
@@ -1008,7 +1005,442 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1495,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
   <dimension ref="A1:V875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1628,7 +2060,7 @@
       <c r="B5" s="18"/>
       <c r="C5" s="16">
         <f ca="1">TODAY()</f>
-        <v>44988</v>
+        <v>44991</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -1678,7 +2110,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
@@ -1772,7 +2204,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="6">
         <v>2</v>
@@ -1961,7 +2393,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23" s="6">
         <v>3</v>
@@ -2131,7 +2563,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="6">
         <v>4</v>
@@ -2251,7 +2683,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B39" s="6">
         <v>5</v>
@@ -2489,7 +2921,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B51" s="6">
         <v>6</v>
@@ -2687,7 +3119,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B61" s="6">
         <v>7</v>
@@ -2817,7 +3249,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" s="6">
         <v>8</v>
@@ -2844,7 +3276,7 @@
         <v>25</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
@@ -2860,7 +3292,7 @@
         <v>21</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
@@ -2876,7 +3308,7 @@
         <v>78</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
@@ -2891,7 +3323,7 @@
         <v>87</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
@@ -2907,7 +3339,7 @@
         <v>85</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -2923,7 +3355,7 @@
         <v>86</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
@@ -2939,7 +3371,7 @@
         <v>80</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
@@ -2955,7 +3387,7 @@
         <v>81</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
@@ -2971,7 +3403,7 @@
         <v>83</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
@@ -2987,24 +3419,24 @@
         <v>84</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B80" s="6">
         <v>9</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D80" s="11"/>
       <c r="E80" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F80" s="11"/>
       <c r="G80" s="9"/>
@@ -3020,7 +3452,7 @@
         <v>25</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -3035,7 +3467,7 @@
         <v>21</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
@@ -3047,10 +3479,10 @@
         <v>3</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
@@ -3062,10 +3494,10 @@
         <v>4</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
@@ -3077,10 +3509,10 @@
         <v>5</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
@@ -3092,10 +3524,10 @@
         <v>6</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
@@ -3107,10 +3539,10 @@
         <v>7</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
@@ -3122,10 +3554,10 @@
         <v>8</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
@@ -3137,10 +3569,10 @@
         <v>9</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
@@ -3152,27 +3584,27 @@
         <v>10</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B91" s="6">
         <v>10</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F91" s="11"/>
       <c r="G91" s="9"/>
@@ -3189,7 +3621,7 @@
         <v>25</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G92" s="8"/>
       <c r="H92" s="8"/>
@@ -3205,7 +3637,7 @@
         <v>21</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G93" s="8"/>
       <c r="H93" s="8"/>
@@ -3218,10 +3650,10 @@
         <v>3</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
@@ -3234,10 +3666,10 @@
         <v>4</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G95" s="8"/>
       <c r="H95" s="8"/>
@@ -3250,10 +3682,10 @@
         <v>5</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -3266,10 +3698,10 @@
         <v>6</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G97" s="8"/>
       <c r="H97" s="8"/>
@@ -3282,10 +3714,10 @@
         <v>7</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
@@ -3298,10 +3730,10 @@
         <v>8</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G99" s="8"/>
       <c r="H99" s="8"/>
@@ -3314,10 +3746,10 @@
         <v>9</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
@@ -11085,31 +11517,101 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F22 F9:F12 F24:F31 F33:F38 F40:F50 F52:F60 F62:F68 F70:F79 F81:F90">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>$F9="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="26" priority="26">
       <formula>$F9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>$F9="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="24" priority="28">
       <formula>$F9="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F92:F101">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="F101">
+    <cfRule type="expression" dxfId="23" priority="21">
+      <formula>$F101="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="22">
+      <formula>$F101="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="23">
+      <formula>$F101="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="24">
+      <formula>$F101="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F92:F96">
+    <cfRule type="expression" dxfId="19" priority="17">
       <formula>$F92="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="18" priority="18">
       <formula>$F92="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>$F92="Failed"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="16" priority="20">
+      <formula>$F92="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F97">
+    <cfRule type="expression" dxfId="15" priority="13">
+      <formula>$F97="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="14">
+      <formula>$F97="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>$F97="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>$F97="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F98">
+    <cfRule type="expression" dxfId="11" priority="9">
+      <formula>$F98="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>$F98="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>$F98="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="12">
+      <formula>$F98="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F99">
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>$F99="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>$F99="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>$F99="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>$F99="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F100">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$F100="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$F100="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$F100="Failed"</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$F92="In work"</formula>
+      <formula>$F100="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -11124,7 +11626,7 @@
           <x14:formula1>
             <xm:f>'Possible results'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F14:F22 F9:F12 F24:F31 F33:F38 F40:F50 F52:F60 F62:F68 F70:F79 F81:F90 F92:F101</xm:sqref>
+          <xm:sqref>F14:F22 F9:F12 F24:F31 F33:F38 F40:F50 F52:F60 F62:F68 F81:F90 F70:F79 F92:F101</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11136,8 +11638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC3EE7E-7188-42AF-B965-808431552D03}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11187,13 +11689,11 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9" s="8" t="s">
-        <v>113</v>
-      </c>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login without UI function added
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C07CB51-F5C7-40BA-8FBC-07A928F531F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3634EE9F-4A23-4B46-BAE6-5D713361679B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="138">
   <si>
     <t>Test plan</t>
   </si>
@@ -698,9 +698,6 @@
     <t>Not as expected - color is white</t>
   </si>
   <si>
-    <t>Otvorit produkt, skontrolovat size a color a ci je mozne pridat do kosika a tiez ci je mozne pridat medzi oblubene bez prihlasenia a potom s prihlasenim</t>
-  </si>
-  <si>
     <t>Pridat produkt do kosika, sidebar sa zobrazi, skontrolovat meno atd, zmenit pocet, odstranit produkt z kosika</t>
   </si>
   <si>
@@ -821,6 +818,21 @@
   </si>
   <si>
     <t>Wishlist should be empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Screen </t>
+  </si>
+  <si>
+    <t>P-001 Product actions</t>
+  </si>
+  <si>
+    <t>Open product and check actions which can be performed on product</t>
+  </si>
+  <si>
+    <t>Otvorit produkt, skontrolovat size a color a ci je mozne pridat medzi oblubene bez prihlasenia - iba UI</t>
+  </si>
+  <si>
+    <t>To iste ale poslat request a na zaklade response skontrolovat ci su zobrazene na stranke dobre udaje</t>
   </si>
 </sst>
 </file>
@@ -1927,8 +1939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
   <dimension ref="A1:V875"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2110,7 +2122,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
@@ -2204,7 +2216,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="6">
         <v>2</v>
@@ -2393,7 +2405,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23" s="6">
         <v>3</v>
@@ -2563,7 +2575,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32" s="6">
         <v>4</v>
@@ -2683,7 +2695,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="6">
         <v>5</v>
@@ -2921,7 +2933,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B51" s="6">
         <v>6</v>
@@ -3119,7 +3131,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B61" s="6">
         <v>7</v>
@@ -3249,7 +3261,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B69" s="6">
         <v>8</v>
@@ -3426,17 +3438,17 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B80" s="6">
         <v>9</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D80" s="11"/>
       <c r="E80" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F80" s="11"/>
       <c r="G80" s="9"/>
@@ -3479,7 +3491,7 @@
         <v>3</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>15</v>
@@ -3494,7 +3506,7 @@
         <v>4</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>15</v>
@@ -3509,7 +3521,7 @@
         <v>5</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>15</v>
@@ -3524,7 +3536,7 @@
         <v>6</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>15</v>
@@ -3539,7 +3551,7 @@
         <v>7</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>15</v>
@@ -3554,7 +3566,7 @@
         <v>8</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>15</v>
@@ -3569,7 +3581,7 @@
         <v>9</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>15</v>
@@ -3584,7 +3596,7 @@
         <v>10</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>15</v>
@@ -3594,17 +3606,17 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B91" s="6">
         <v>10</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F91" s="11"/>
       <c r="G91" s="9"/>
@@ -3650,7 +3662,7 @@
         <v>3</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>15</v>
@@ -3666,7 +3678,7 @@
         <v>4</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>15</v>
@@ -3682,7 +3694,7 @@
         <v>5</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>15</v>
@@ -3698,7 +3710,7 @@
         <v>6</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>15</v>
@@ -3714,7 +3726,7 @@
         <v>7</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>15</v>
@@ -3730,7 +3742,7 @@
         <v>8</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>15</v>
@@ -3746,7 +3758,7 @@
         <v>9</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>15</v>
@@ -3755,14 +3767,22 @@
       <c r="H100" s="8"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="8"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="8"/>
+      <c r="A101" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B101" s="6">
+        <v>1</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D101" s="11"/>
+      <c r="E101" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F101" s="11"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="8"/>
@@ -11528,20 +11548,6 @@
     </cfRule>
     <cfRule type="expression" dxfId="24" priority="28">
       <formula>$F9="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F101">
-    <cfRule type="expression" dxfId="23" priority="21">
-      <formula>$F101="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="22">
-      <formula>$F101="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="23">
-      <formula>$F101="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="24">
-      <formula>$F101="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F92:F96">
@@ -11626,7 +11632,7 @@
           <x14:formula1>
             <xm:f>'Possible results'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F14:F22 F9:F12 F24:F31 F33:F38 F40:F50 F52:F60 F62:F68 F81:F90 F70:F79 F92:F101</xm:sqref>
+          <xm:sqref>F14:F22 F9:F12 F24:F31 F33:F38 F40:F50 F52:F60 F62:F68 F81:F90 F70:F79 F92:F100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11639,7 +11645,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11660,32 +11666,31 @@
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="8" t="s">
-        <v>109</v>
+      <c r="C4" s="8" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -11693,7 +11698,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First product test in progress
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3634EE9F-4A23-4B46-BAE6-5D713361679B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFD39E6-FA51-4E29-8DB5-2F65BF1BB01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="132">
   <si>
     <t>Test plan</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Page successfully opened</t>
   </si>
   <si>
-    <t>URL contains localhost:3000 and title contains ACME Storefront</t>
-  </si>
-  <si>
     <t>As expected</t>
   </si>
   <si>
@@ -137,22 +134,10 @@
     <t>Move mouse to each of the images in upper grid</t>
   </si>
   <si>
-    <t>Check correctness of URL and title</t>
-  </si>
-  <si>
-    <t>Check that upper grid contains 3 products</t>
-  </si>
-  <si>
-    <t>Check that images get bigger on hover</t>
-  </si>
-  <si>
     <t>Check if shopify info part contains correct header and content</t>
   </si>
   <si>
     <t>Scroll down to see information part about Shopify</t>
-  </si>
-  <si>
-    <t>Check that it contains correct header and content</t>
   </si>
   <si>
     <r>
@@ -186,9 +171,6 @@
     <t>Scroll down to lower product grid</t>
   </si>
   <si>
-    <t>Check that lower grid contains 3 products</t>
-  </si>
-  <si>
     <t>Check links in footer redirect user to correct pages</t>
   </si>
   <si>
@@ -254,23 +236,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Check if user is correctly redirected to </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>vercel.com/contact</t>
-    </r>
-  </si>
-  <si>
     <t>Check if background changing function is working correctly</t>
   </si>
   <si>
@@ -294,12 +259,6 @@
     <t>Change website background to System</t>
   </si>
   <si>
-    <t>Check if background is in correct color - white</t>
-  </si>
-  <si>
-    <t>Check if background is in correct color - black</t>
-  </si>
-  <si>
     <t>Change website background to Dark</t>
   </si>
   <si>
@@ -309,33 +268,21 @@
     <t>Change website language to Espanyol</t>
   </si>
   <si>
-    <t>Check if language is successfully changed</t>
-  </si>
-  <si>
     <t>Change website language to English</t>
   </si>
   <si>
     <t>Click on GitHub logo</t>
   </si>
   <si>
-    <t>Check if user is redirected to Vercel GitHub</t>
-  </si>
-  <si>
     <t>H-003 Sliders products count</t>
   </si>
   <si>
     <t>Check if upper slider contains 3 products and lower slider 1 product</t>
   </si>
   <si>
-    <t>Check that upper slider contains 3 products</t>
-  </si>
-  <si>
     <t>Scroll down to see the lower slider</t>
   </si>
   <si>
-    <t>Check that lower slider contains 1 product</t>
-  </si>
-  <si>
     <t>H-004 Shopify information header and content</t>
   </si>
   <si>
@@ -348,21 +295,9 @@
     <t>Check if each of the grids contain 3 products and check image hover effect</t>
   </si>
   <si>
-    <t>Upper grid contains 3 products</t>
-  </si>
-  <si>
     <t>Hover effect is working properly</t>
   </si>
   <si>
-    <t>Lower product grid is visible</t>
-  </si>
-  <si>
-    <t>Each of the images is visible</t>
-  </si>
-  <si>
-    <t>Lower grid contains 3 products</t>
-  </si>
-  <si>
     <t>H-002 Grid products count and effect</t>
   </si>
   <si>
@@ -373,46 +308,6 @@
   </si>
   <si>
     <t>Cookies banner is not visible (cookies are accepted before each test case)</t>
-  </si>
-  <si>
-    <t>Check that upper slider contains: Train&amp;Sleep T-shirt, Nike T-shirt, QR code</t>
-  </si>
-  <si>
-    <t>Check that lower slider contains: Code Shirt</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Check if user is redirected to </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>shopify.vercel.store</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Check if user is correctly redirected to </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>shopify.vercel.store</t>
-    </r>
   </si>
   <si>
     <t>H-005 Link redirections in footer</t>
@@ -446,38 +341,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Show all products by clicking on button </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>All</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> and order them by different options</t>
-    </r>
-  </si>
-  <si>
-    <t>In option Price: Low to high check that prices are in ascending order</t>
-  </si>
-  <si>
-    <t>In option Price: High to low check that prices are in descending order</t>
-  </si>
-  <si>
     <t>H-008 Show all products and order them</t>
   </si>
   <si>
@@ -509,62 +372,6 @@
     </r>
   </si>
   <si>
-    <t>Check that page contains 2 products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check that page contains 4 products </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check that page contains just products from list </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Check that URL contains word </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>search</t>
-    </r>
-  </si>
-  <si>
-    <t>Scroll down to see the slider</t>
-  </si>
-  <si>
-    <t>Upper slider contains 3 products</t>
-  </si>
-  <si>
-    <t>Upper slider contains correct product names</t>
-  </si>
-  <si>
-    <t>Lower slider is visible</t>
-  </si>
-  <si>
-    <t>Upper slider is visible</t>
-  </si>
-  <si>
-    <t>Upper slider contains 1 product</t>
-  </si>
-  <si>
-    <t>Upper slider contains correct product name</t>
-  </si>
-  <si>
-    <t>Information part is visible</t>
-  </si>
-  <si>
-    <t>Header and content is correct</t>
-  </si>
-  <si>
-    <t>Website is correctly displayed</t>
-  </si>
-  <si>
     <t>Footer is visible</t>
   </si>
   <si>
@@ -683,21 +490,6 @@
     </r>
   </si>
   <si>
-    <t>Background successfully changed</t>
-  </si>
-  <si>
-    <t>Not as expected - color is blue</t>
-  </si>
-  <si>
-    <t>Background color is white</t>
-  </si>
-  <si>
-    <t>Background color is black</t>
-  </si>
-  <si>
-    <t>Not as expected - color is white</t>
-  </si>
-  <si>
     <t>Pridat produkt do kosika, sidebar sa zobrazi, skontrolovat meno atd, zmenit pocet, odstranit produkt z kosika</t>
   </si>
   <si>
@@ -711,9 +503,6 @@
   </si>
   <si>
     <t xml:space="preserve">Home Screen </t>
-  </si>
-  <si>
-    <t>Click inside search bar</t>
   </si>
   <si>
     <r>
@@ -744,12 +533,6 @@
     </r>
   </si>
   <si>
-    <t>Check label in searched products</t>
-  </si>
-  <si>
-    <t>Check product count</t>
-  </si>
-  <si>
     <t>H-009 Search for product</t>
   </si>
   <si>
@@ -833,6 +616,260 @@
   </si>
   <si>
     <t>To iste ale poslat request a na zaklade response skontrolovat ci su zobrazene na stranke dobre udaje</t>
+  </si>
+  <si>
+    <t>Registracia testy</t>
+  </si>
+  <si>
+    <t>Open first product in upper grid</t>
+  </si>
+  <si>
+    <t>Click on Care button</t>
+  </si>
+  <si>
+    <t>Collapsed content should be visible</t>
+  </si>
+  <si>
+    <t>Click on Details button</t>
+  </si>
+  <si>
+    <t>In "empty" state Care and Details content should not be visible</t>
+  </si>
+  <si>
+    <t>Open second product in upper grid</t>
+  </si>
+  <si>
+    <t>Select size that is not available</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add to cart button should be disabled with text </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Not available</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> and cursor should be disabled</t>
+    </r>
+  </si>
+  <si>
+    <t>Background successfully changed to White</t>
+  </si>
+  <si>
+    <t>Background successfully changed to Black</t>
+  </si>
+  <si>
+    <t>Order products by option Price: Low to High</t>
+  </si>
+  <si>
+    <t>Order products by option Price: High to Low</t>
+  </si>
+  <si>
+    <t>Check founded product (label and product count)</t>
+  </si>
+  <si>
+    <t>URL should contain localhost:3000 and title ACME Storefront</t>
+  </si>
+  <si>
+    <t>Page successfully opened, upper grid should contain 3 products</t>
+  </si>
+  <si>
+    <t>Lower product grid is visible and contains 3 products</t>
+  </si>
+  <si>
+    <t>Upper slider is visible and contains 3 products with correct names</t>
+  </si>
+  <si>
+    <t>Lower slider is visible and contains 1 product with correct name</t>
+  </si>
+  <si>
+    <t>Scroll down to see the upper slider</t>
+  </si>
+  <si>
+    <t>Information part is visible with correct header and content</t>
+  </si>
+  <si>
+    <t>Website language successfully changed to Espanyol</t>
+  </si>
+  <si>
+    <t>Website language successfully changed to English</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Show all products by clicking on button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>All</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> and order them</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Url should contain word </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>, page should contain 4 products with correct names</t>
+    </r>
+  </si>
+  <si>
+    <t>Page should contain 2 products with correct names</t>
+  </si>
+  <si>
+    <t>Product prices should be ordered ascending</t>
+  </si>
+  <si>
+    <t>Product prices should be ordered descending</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Search bar contains word </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Nike</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">Search page contains 1 product with </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">Nike </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>inside his name</t>
+    </r>
+  </si>
+  <si>
+    <t>Search bar is empty</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Search bar contains word </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Test</t>
+    </r>
+  </si>
+  <si>
+    <t>Search page does not contain any found products</t>
+  </si>
+  <si>
+    <t>User successfully logged in</t>
+  </si>
+  <si>
+    <t>Product page successfully opened</t>
+  </si>
+  <si>
+    <t>Try every possible actions on product page</t>
+  </si>
+  <si>
+    <t>Every color should be clickable and is possible to add it to cart</t>
+  </si>
+  <si>
+    <t>Try additional info actions on product page</t>
+  </si>
+  <si>
+    <t>Home page is displayed</t>
+  </si>
+  <si>
+    <t>Product page successfully opened, product name is correct and also URL is correct</t>
   </si>
 </sst>
 </file>
@@ -960,7 +997,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -991,6 +1028,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1017,7 +1055,442 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1937,10 +2410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
-  <dimension ref="A1:V875"/>
+  <dimension ref="A1:V845"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1951,148 +2424,148 @@
     <col min="4" max="4" width="6.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="63.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="62.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="16">
+      <c r="B5" s="19"/>
+      <c r="C5" s="17">
         <f ca="1">TODAY()</f>
-        <v>44991</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
+        <v>44993</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
     </row>
     <row r="7" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -2122,13 +2595,13 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="9" t="s">
@@ -2145,16 +2618,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
@@ -2170,10 +2643,10 @@
         <v>13</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -2183,266 +2656,261 @@
         <v>3</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="8" t="s">
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="6">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7">
-        <v>4</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" s="6">
-        <v>2</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="G13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="7">
-        <v>5</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="6">
+        <v>3</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="B23" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="9" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="C24" s="8"/>
       <c r="D24" s="7">
         <v>1</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="C25" s="8"/>
       <c r="D25" s="7">
         <v>2</v>
       </c>
@@ -2456,279 +2924,297 @@
         <v>22</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="C26" s="8"/>
       <c r="D26" s="7">
         <v>3</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="C27" s="8"/>
       <c r="D27" s="7">
         <v>4</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="7">
+      <c r="A28" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="6">
         <v>5</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="C28" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B32" s="6">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="7">
         <v>4</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+      <c r="E32" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
       <c r="D34" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
       <c r="D36" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="H36" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="6">
+        <v>6</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7">
+        <v>1</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D37" s="7">
-        <v>5</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D38" s="7">
-        <v>6</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="6">
-        <v>5</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F39" s="11"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7">
+        <v>2</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2736,19 +3222,19 @@
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2756,7 +3242,7 @@
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>38</v>
@@ -2765,10 +3251,10 @@
         <v>13</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2776,7 +3262,7 @@
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>39</v>
@@ -2785,462 +3271,434 @@
         <v>13</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="2">
-        <v>5</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A44" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="6">
+        <v>7</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="11"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="2">
-        <v>6</v>
+      <c r="D45" s="7">
+        <v>1</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H45" s="8"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="2">
-        <v>7</v>
+      <c r="D46" s="7">
+        <v>2</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="2">
-        <v>8</v>
+      <c r="D47" s="7">
+        <v>3</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="2">
-        <v>9</v>
+      <c r="D48" s="7">
+        <v>4</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="2">
-        <v>10</v>
+      <c r="D49" s="7">
+        <v>5</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H49" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="6">
+        <v>8</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="11"/>
+      <c r="E50" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="7">
+        <v>1</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="2">
-        <v>11</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="6">
-        <v>6</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
+      <c r="F51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51" s="8"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="2">
-        <v>5</v>
+      <c r="D56" s="7">
+        <v>6</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>105</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="2">
-        <v>6</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A57" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="6">
+        <v>9</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
       <c r="D58" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>108</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
       <c r="D59" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H59" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
       <c r="D60" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H60" s="8" t="s">
-        <v>108</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="H60" s="8"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="6">
-        <v>7</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D61" s="11"/>
-      <c r="E61" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="D61" s="2">
+        <v>5</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="7">
-        <v>1</v>
+      <c r="D62" s="2">
+        <v>6</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G62" s="8"/>
+      <c r="G62" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="7">
-        <v>2</v>
+      <c r="D63" s="2">
+        <v>7</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G63" s="8"/>
+      <c r="G63" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="H63" s="8"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="7">
-        <v>3</v>
+      <c r="D64" s="2">
+        <v>8</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G64" s="8"/>
+      <c r="G64" s="8" t="s">
+        <v>123</v>
+      </c>
       <c r="H64" s="8"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="7">
-        <v>4</v>
+      <c r="D65" s="2">
+        <v>9</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G65" s="8"/>
+      <c r="G65" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="H65" s="8"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="2">
-        <v>5</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
+      <c r="A66" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="6">
+        <v>10</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" s="11"/>
+      <c r="E66" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F66" s="11"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G67" s="8"/>
+      <c r="G67" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H67" s="8"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -3248,393 +3706,400 @@
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
       <c r="D68" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G68" s="8"/>
+      <c r="G68" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B69" s="6">
-        <v>8</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D69" s="11"/>
-      <c r="E69" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F69" s="11"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="2">
+        <v>3</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H69" s="8"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="7">
-        <v>1</v>
+      <c r="D70" s="2">
+        <v>5</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G70" s="8"/>
+      <c r="G70" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="7">
-        <v>2</v>
+      <c r="D71" s="2">
+        <v>6</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G71" s="8"/>
+      <c r="G71" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="H71" s="8"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="7">
-        <v>3</v>
+      <c r="D72" s="2">
+        <v>7</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G72" s="8"/>
+      <c r="G72" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="H72" s="8"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
-      <c r="D73" s="7">
-        <v>4</v>
-      </c>
-      <c r="E73" s="8" t="s">
+      <c r="A73" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
+      <c r="B73" s="6">
+        <v>1</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D73" s="11"/>
+      <c r="E73" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F73" s="11"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="7">
-        <v>5</v>
+      <c r="D74" s="2">
+        <v>1</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G74" s="8"/>
+      <c r="G74" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H74" s="8"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="7">
-        <v>6</v>
+      <c r="D75" s="2">
+        <v>2</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G75" s="8"/>
+      <c r="G75" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H75" s="8"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="7">
-        <v>7</v>
+      <c r="D76" s="2">
+        <v>3</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G76" s="8"/>
+      <c r="G76" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="H76" s="8"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="7">
-        <v>8</v>
+      <c r="D77" s="2">
+        <v>4</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G77" s="8"/>
+      <c r="G77" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="H77" s="8"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="7">
-        <v>9</v>
+      <c r="D78" s="2">
+        <v>5</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G78" s="8"/>
+      <c r="G78" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="H78" s="8"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="7">
-        <v>10</v>
+      <c r="D79" s="2">
+        <v>6</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G79" s="8"/>
+      <c r="G79" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="H79" s="8"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A80" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B80" s="6">
-        <v>9</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D80" s="11"/>
-      <c r="E80" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F80" s="11"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="2">
+        <v>7</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H80" s="8"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
       <c r="D81" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G81" s="8"/>
+      <c r="G81" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="H81" s="8"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
       <c r="D82" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G82" s="8"/>
+      <c r="G82" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="H82" s="8"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
       <c r="D83" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G83" s="8"/>
+      <c r="G83" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="H83" s="8"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
       <c r="D84" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G84" s="8"/>
+      <c r="G84" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="H84" s="8"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
       <c r="D85" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G85" s="8"/>
+      <c r="G85" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="H85" s="8"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
       <c r="D86" s="2">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G86" s="8"/>
+      <c r="G86" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="H86" s="8"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
-      <c r="D87" s="2">
-        <v>7</v>
-      </c>
-      <c r="E87" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C87" s="8"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
-      <c r="D88" s="2">
-        <v>8</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
       <c r="B89" s="8"/>
-      <c r="D89" s="2">
-        <v>9</v>
-      </c>
-      <c r="E89" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C89" s="8"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="8"/>
       <c r="B90" s="8"/>
-      <c r="D90" s="2">
-        <v>10</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B91" s="6">
-        <v>10</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D91" s="11"/>
-      <c r="E91" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F91" s="11"/>
-      <c r="G91" s="9"/>
-      <c r="H91" s="9"/>
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="8"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
-      <c r="D92" s="2">
-        <v>1</v>
-      </c>
-      <c r="E92" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
       <c r="G92" s="8"/>
       <c r="H92" s="8"/>
     </row>
@@ -3642,15 +4107,9 @@
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
-      <c r="D93" s="2">
-        <v>2</v>
-      </c>
-      <c r="E93" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
       <c r="G93" s="8"/>
       <c r="H93" s="8"/>
     </row>
@@ -3658,15 +4117,9 @@
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
-      <c r="D94" s="2">
-        <v>3</v>
-      </c>
-      <c r="E94" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
     </row>
@@ -3674,15 +4127,9 @@
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
-      <c r="D95" s="2">
-        <v>4</v>
-      </c>
-      <c r="E95" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
       <c r="G95" s="8"/>
       <c r="H95" s="8"/>
     </row>
@@ -3690,15 +4137,9 @@
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="2">
-        <v>5</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
     </row>
@@ -3706,15 +4147,9 @@
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="2">
-        <v>6</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="8"/>
       <c r="G97" s="8"/>
       <c r="H97" s="8"/>
     </row>
@@ -3722,15 +4157,9 @@
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="2">
-        <v>7</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="8"/>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
     </row>
@@ -3738,15 +4167,9 @@
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
-      <c r="D99" s="2">
-        <v>8</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
       <c r="G99" s="8"/>
       <c r="H99" s="8"/>
     </row>
@@ -3754,35 +4177,21 @@
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
-      <c r="D100" s="2">
-        <v>9</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B101" s="6">
-        <v>1</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D101" s="11"/>
-      <c r="E101" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="F101" s="11"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="9"/>
+      <c r="A101" s="8"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="8"/>
@@ -11223,306 +11632,6 @@
       <c r="F845" s="8"/>
       <c r="G845" s="8"/>
       <c r="H845" s="8"/>
-    </row>
-    <row r="846" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A846" s="8"/>
-      <c r="B846" s="8"/>
-      <c r="C846" s="8"/>
-      <c r="D846" s="2"/>
-      <c r="E846" s="8"/>
-      <c r="F846" s="8"/>
-      <c r="G846" s="8"/>
-      <c r="H846" s="8"/>
-    </row>
-    <row r="847" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A847" s="8"/>
-      <c r="B847" s="8"/>
-      <c r="C847" s="8"/>
-      <c r="D847" s="2"/>
-      <c r="E847" s="8"/>
-      <c r="F847" s="8"/>
-      <c r="G847" s="8"/>
-      <c r="H847" s="8"/>
-    </row>
-    <row r="848" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A848" s="8"/>
-      <c r="B848" s="8"/>
-      <c r="C848" s="8"/>
-      <c r="D848" s="2"/>
-      <c r="E848" s="8"/>
-      <c r="F848" s="8"/>
-      <c r="G848" s="8"/>
-      <c r="H848" s="8"/>
-    </row>
-    <row r="849" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A849" s="8"/>
-      <c r="B849" s="8"/>
-      <c r="C849" s="8"/>
-      <c r="D849" s="2"/>
-      <c r="E849" s="8"/>
-      <c r="F849" s="8"/>
-      <c r="G849" s="8"/>
-      <c r="H849" s="8"/>
-    </row>
-    <row r="850" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A850" s="8"/>
-      <c r="B850" s="8"/>
-      <c r="C850" s="8"/>
-      <c r="D850" s="2"/>
-      <c r="E850" s="8"/>
-      <c r="F850" s="8"/>
-      <c r="G850" s="8"/>
-      <c r="H850" s="8"/>
-    </row>
-    <row r="851" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A851" s="8"/>
-      <c r="B851" s="8"/>
-      <c r="C851" s="8"/>
-      <c r="D851" s="2"/>
-      <c r="E851" s="8"/>
-      <c r="F851" s="8"/>
-      <c r="G851" s="8"/>
-      <c r="H851" s="8"/>
-    </row>
-    <row r="852" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A852" s="8"/>
-      <c r="B852" s="8"/>
-      <c r="C852" s="8"/>
-      <c r="D852" s="2"/>
-      <c r="E852" s="8"/>
-      <c r="F852" s="8"/>
-      <c r="G852" s="8"/>
-      <c r="H852" s="8"/>
-    </row>
-    <row r="853" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A853" s="8"/>
-      <c r="B853" s="8"/>
-      <c r="C853" s="8"/>
-      <c r="D853" s="2"/>
-      <c r="E853" s="8"/>
-      <c r="F853" s="8"/>
-      <c r="G853" s="8"/>
-      <c r="H853" s="8"/>
-    </row>
-    <row r="854" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A854" s="8"/>
-      <c r="B854" s="8"/>
-      <c r="C854" s="8"/>
-      <c r="D854" s="2"/>
-      <c r="E854" s="8"/>
-      <c r="F854" s="8"/>
-      <c r="G854" s="8"/>
-      <c r="H854" s="8"/>
-    </row>
-    <row r="855" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A855" s="8"/>
-      <c r="B855" s="8"/>
-      <c r="C855" s="8"/>
-      <c r="D855" s="2"/>
-      <c r="E855" s="8"/>
-      <c r="F855" s="8"/>
-      <c r="G855" s="8"/>
-      <c r="H855" s="8"/>
-    </row>
-    <row r="856" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A856" s="8"/>
-      <c r="B856" s="8"/>
-      <c r="C856" s="8"/>
-      <c r="D856" s="2"/>
-      <c r="E856" s="8"/>
-      <c r="F856" s="8"/>
-      <c r="G856" s="8"/>
-      <c r="H856" s="8"/>
-    </row>
-    <row r="857" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A857" s="8"/>
-      <c r="B857" s="8"/>
-      <c r="C857" s="8"/>
-      <c r="D857" s="2"/>
-      <c r="E857" s="8"/>
-      <c r="F857" s="8"/>
-      <c r="G857" s="8"/>
-      <c r="H857" s="8"/>
-    </row>
-    <row r="858" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A858" s="8"/>
-      <c r="B858" s="8"/>
-      <c r="C858" s="8"/>
-      <c r="D858" s="2"/>
-      <c r="E858" s="8"/>
-      <c r="F858" s="8"/>
-      <c r="G858" s="8"/>
-      <c r="H858" s="8"/>
-    </row>
-    <row r="859" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A859" s="8"/>
-      <c r="B859" s="8"/>
-      <c r="C859" s="8"/>
-      <c r="D859" s="2"/>
-      <c r="E859" s="8"/>
-      <c r="F859" s="8"/>
-      <c r="G859" s="8"/>
-      <c r="H859" s="8"/>
-    </row>
-    <row r="860" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A860" s="8"/>
-      <c r="B860" s="8"/>
-      <c r="C860" s="8"/>
-      <c r="D860" s="2"/>
-      <c r="E860" s="8"/>
-      <c r="F860" s="8"/>
-      <c r="G860" s="8"/>
-      <c r="H860" s="8"/>
-    </row>
-    <row r="861" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A861" s="8"/>
-      <c r="B861" s="8"/>
-      <c r="C861" s="8"/>
-      <c r="D861" s="2"/>
-      <c r="E861" s="8"/>
-      <c r="F861" s="8"/>
-      <c r="G861" s="8"/>
-      <c r="H861" s="8"/>
-    </row>
-    <row r="862" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A862" s="8"/>
-      <c r="B862" s="8"/>
-      <c r="C862" s="8"/>
-      <c r="D862" s="2"/>
-      <c r="E862" s="8"/>
-      <c r="F862" s="8"/>
-      <c r="G862" s="8"/>
-      <c r="H862" s="8"/>
-    </row>
-    <row r="863" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A863" s="8"/>
-      <c r="B863" s="8"/>
-      <c r="C863" s="8"/>
-      <c r="D863" s="2"/>
-      <c r="E863" s="8"/>
-      <c r="F863" s="8"/>
-      <c r="G863" s="8"/>
-      <c r="H863" s="8"/>
-    </row>
-    <row r="864" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A864" s="8"/>
-      <c r="B864" s="8"/>
-      <c r="C864" s="8"/>
-      <c r="D864" s="2"/>
-      <c r="E864" s="8"/>
-      <c r="F864" s="8"/>
-      <c r="G864" s="8"/>
-      <c r="H864" s="8"/>
-    </row>
-    <row r="865" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A865" s="8"/>
-      <c r="B865" s="8"/>
-      <c r="C865" s="8"/>
-      <c r="D865" s="2"/>
-      <c r="E865" s="8"/>
-      <c r="F865" s="8"/>
-      <c r="G865" s="8"/>
-      <c r="H865" s="8"/>
-    </row>
-    <row r="866" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A866" s="8"/>
-      <c r="B866" s="8"/>
-      <c r="C866" s="8"/>
-      <c r="D866" s="2"/>
-      <c r="E866" s="8"/>
-      <c r="F866" s="8"/>
-      <c r="G866" s="8"/>
-      <c r="H866" s="8"/>
-    </row>
-    <row r="867" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A867" s="8"/>
-      <c r="B867" s="8"/>
-      <c r="C867" s="8"/>
-      <c r="D867" s="2"/>
-      <c r="E867" s="8"/>
-      <c r="F867" s="8"/>
-      <c r="G867" s="8"/>
-      <c r="H867" s="8"/>
-    </row>
-    <row r="868" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A868" s="8"/>
-      <c r="B868" s="8"/>
-      <c r="C868" s="8"/>
-      <c r="D868" s="2"/>
-      <c r="E868" s="8"/>
-      <c r="F868" s="8"/>
-      <c r="G868" s="8"/>
-      <c r="H868" s="8"/>
-    </row>
-    <row r="869" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A869" s="8"/>
-      <c r="B869" s="8"/>
-      <c r="C869" s="8"/>
-      <c r="D869" s="2"/>
-      <c r="E869" s="8"/>
-      <c r="F869" s="8"/>
-      <c r="G869" s="8"/>
-      <c r="H869" s="8"/>
-    </row>
-    <row r="870" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A870" s="8"/>
-      <c r="B870" s="8"/>
-      <c r="C870" s="8"/>
-      <c r="D870" s="2"/>
-      <c r="E870" s="8"/>
-      <c r="F870" s="8"/>
-      <c r="G870" s="8"/>
-      <c r="H870" s="8"/>
-    </row>
-    <row r="871" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A871" s="8"/>
-      <c r="B871" s="8"/>
-      <c r="C871" s="8"/>
-      <c r="D871" s="2"/>
-      <c r="E871" s="8"/>
-      <c r="F871" s="8"/>
-      <c r="G871" s="8"/>
-      <c r="H871" s="8"/>
-    </row>
-    <row r="872" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A872" s="8"/>
-      <c r="B872" s="8"/>
-      <c r="C872" s="8"/>
-      <c r="D872" s="2"/>
-      <c r="E872" s="8"/>
-      <c r="F872" s="8"/>
-      <c r="G872" s="8"/>
-      <c r="H872" s="8"/>
-    </row>
-    <row r="873" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A873" s="8"/>
-      <c r="B873" s="8"/>
-      <c r="C873" s="8"/>
-      <c r="D873" s="2"/>
-      <c r="E873" s="8"/>
-      <c r="F873" s="8"/>
-      <c r="G873" s="8"/>
-      <c r="H873" s="8"/>
-    </row>
-    <row r="874" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A874" s="8"/>
-      <c r="B874" s="8"/>
-      <c r="C874" s="8"/>
-      <c r="D874" s="2"/>
-      <c r="E874" s="8"/>
-      <c r="F874" s="8"/>
-      <c r="G874" s="8"/>
-      <c r="H874" s="8"/>
-    </row>
-    <row r="875" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A875" s="8"/>
-      <c r="B875" s="8"/>
-      <c r="C875" s="8"/>
-      <c r="D875" s="2"/>
-      <c r="E875" s="8"/>
-      <c r="F875" s="8"/>
-      <c r="G875" s="8"/>
-      <c r="H875" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -11536,88 +11645,144 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F14:F22 F9:F12 F24:F31 F33:F38 F40:F50 F52:F60 F62:F68 F70:F79 F81:F90">
-    <cfRule type="expression" dxfId="27" priority="25">
+  <conditionalFormatting sqref="F38:F43 F45:F49 F67:F70 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65">
+    <cfRule type="expression" dxfId="47" priority="61">
       <formula>$F9="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="26">
+    <cfRule type="expression" dxfId="46" priority="62">
       <formula>$F9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="45" priority="63">
       <formula>$F9="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="28">
+    <cfRule type="expression" dxfId="44" priority="64">
       <formula>$F9="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F92:F96">
-    <cfRule type="expression" dxfId="19" priority="17">
-      <formula>$F92="Open"</formula>
+  <conditionalFormatting sqref="F71">
+    <cfRule type="expression" dxfId="43" priority="49">
+      <formula>$F71="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
-      <formula>$F92="Passed"</formula>
+    <cfRule type="expression" dxfId="42" priority="50">
+      <formula>$F71="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="19">
-      <formula>$F92="Failed"</formula>
+    <cfRule type="expression" dxfId="41" priority="51">
+      <formula>$F71="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
-      <formula>$F92="In work"</formula>
+    <cfRule type="expression" dxfId="40" priority="52">
+      <formula>$F71="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F97">
+  <conditionalFormatting sqref="F72">
+    <cfRule type="expression" dxfId="39" priority="41">
+      <formula>$F72="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="42">
+      <formula>$F72="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="43">
+      <formula>$F72="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="44">
+      <formula>$F72="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F74:F77">
+    <cfRule type="expression" dxfId="35" priority="33">
+      <formula>$F74="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="34">
+      <formula>$F74="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="35">
+      <formula>$F74="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="36">
+      <formula>$F74="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F78">
+    <cfRule type="expression" dxfId="31" priority="29">
+      <formula>$F78="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="30">
+      <formula>$F78="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="31">
+      <formula>$F78="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="32">
+      <formula>$F78="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F79">
+    <cfRule type="expression" dxfId="27" priority="25">
+      <formula>$F79="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="26">
+      <formula>$F79="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="27">
+      <formula>$F79="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="28">
+      <formula>$F79="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F86">
     <cfRule type="expression" dxfId="15" priority="13">
-      <formula>$F97="Open"</formula>
+      <formula>$F86="Open"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="14" priority="14">
-      <formula>$F97="Passed"</formula>
+      <formula>$F86="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="15">
-      <formula>$F97="Failed"</formula>
+      <formula>$F86="Failed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="16">
-      <formula>$F97="In work"</formula>
+      <formula>$F86="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F98">
+  <conditionalFormatting sqref="F80:F83">
     <cfRule type="expression" dxfId="11" priority="9">
-      <formula>$F98="Open"</formula>
+      <formula>$F80="Open"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="10">
-      <formula>$F98="Passed"</formula>
+      <formula>$F80="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="11">
-      <formula>$F98="Failed"</formula>
+      <formula>$F80="Failed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="12">
-      <formula>$F98="In work"</formula>
+      <formula>$F80="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F99">
+  <conditionalFormatting sqref="F84">
     <cfRule type="expression" dxfId="7" priority="5">
-      <formula>$F99="Open"</formula>
+      <formula>$F84="Open"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$F99="Passed"</formula>
+      <formula>$F84="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="7">
-      <formula>$F99="Failed"</formula>
+      <formula>$F84="Failed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="8">
-      <formula>$F99="In work"</formula>
+      <formula>$F84="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F100">
+  <conditionalFormatting sqref="F85">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$F100="Open"</formula>
+      <formula>$F85="Open"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$F100="Passed"</formula>
+      <formula>$F85="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$F100="Failed"</formula>
+      <formula>$F85="Failed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$F100="In work"</formula>
+      <formula>$F85="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -11632,7 +11797,7 @@
           <x14:formula1>
             <xm:f>'Possible results'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F14:F22 F9:F12 F24:F31 F33:F38 F40:F50 F52:F60 F62:F68 F81:F90 F70:F79 F92:F100</xm:sqref>
+          <xm:sqref>F38:F43 F45:F49 F67:F72 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65 F74:F86</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11644,8 +11809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC3EE7E-7188-42AF-B965-808431552D03}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11667,7 +11832,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -11675,30 +11840,32 @@
         <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" s="8" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" s="8" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Product suite test case 2 added + comments added
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFD39E6-FA51-4E29-8DB5-2F65BF1BB01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71350A99-87EA-4473-9614-B8B84A554274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="129">
   <si>
     <t>Test plan</t>
   </si>
@@ -606,15 +606,9 @@
     <t xml:space="preserve">Product Screen </t>
   </si>
   <si>
-    <t>P-001 Product actions</t>
-  </si>
-  <si>
     <t>Open product and check actions which can be performed on product</t>
   </si>
   <si>
-    <t>Otvorit produkt, skontrolovat size a color a ci je mozne pridat medzi oblubene bez prihlasenia - iba UI</t>
-  </si>
-  <si>
     <t>To iste ale poslat request a na zaklade response skontrolovat ci su zobrazene na stranke dobre udaje</t>
   </si>
   <si>
@@ -637,37 +631,6 @@
   </si>
   <si>
     <t>Open second product in upper grid</t>
-  </si>
-  <si>
-    <t>Select size that is not available</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Add to cart button should be disabled with text </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>Not available</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> and cursor should be disabled</t>
-    </r>
   </si>
   <si>
     <t>Background successfully changed to White</t>
@@ -854,9 +817,6 @@
     <t>User successfully logged in</t>
   </si>
   <si>
-    <t>Product page successfully opened</t>
-  </si>
-  <si>
     <t>Try every possible actions on product page</t>
   </si>
   <si>
@@ -866,10 +826,16 @@
     <t>Try additional info actions on product page</t>
   </si>
   <si>
-    <t>Home page is displayed</t>
-  </si>
-  <si>
     <t>Product page successfully opened, product name is correct and also URL is correct</t>
+  </si>
+  <si>
+    <t>P-001 Product actions with color options</t>
+  </si>
+  <si>
+    <t>P-002 Product actions with sizes options</t>
+  </si>
+  <si>
+    <t>Last size is not possible to add to cart</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1021,181 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2410,10 +2550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
-  <dimension ref="A1:V845"/>
+  <dimension ref="A1:V842"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2545,7 +2685,7 @@
       <c r="B5" s="19"/>
       <c r="C5" s="17">
         <f ca="1">TODAY()</f>
-        <v>44993</v>
+        <v>45005</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -2643,7 +2783,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>23</v>
@@ -2718,7 +2858,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>23</v>
@@ -2756,7 +2896,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>23</v>
@@ -2844,13 +2984,13 @@
         <v>3</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>23</v>
@@ -2869,7 +3009,7 @@
         <v>13</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>23</v>
@@ -2938,7 +3078,7 @@
         <v>13</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>23</v>
@@ -3231,7 +3371,7 @@
         <v>13</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>23</v>
@@ -3251,7 +3391,7 @@
         <v>13</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>23</v>
@@ -3271,7 +3411,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>23</v>
@@ -3363,7 +3503,7 @@
         <v>15</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H48" s="8"/>
     </row>
@@ -3381,7 +3521,7 @@
         <v>15</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H49" s="8"/>
     </row>
@@ -3397,7 +3537,7 @@
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F50" s="11"/>
       <c r="G50" s="9"/>
@@ -3453,7 +3593,7 @@
         <v>15</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H53" s="8"/>
     </row>
@@ -3465,13 +3605,13 @@
         <v>4</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H54" s="8"/>
     </row>
@@ -3483,13 +3623,13 @@
         <v>5</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H55" s="8"/>
     </row>
@@ -3507,7 +3647,7 @@
         <v>15</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H56" s="8"/>
     </row>
@@ -3576,7 +3716,7 @@
         <v>15</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H60" s="8"/>
     </row>
@@ -3587,13 +3727,13 @@
         <v>5</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H61" s="8"/>
     </row>
@@ -3627,7 +3767,7 @@
         <v>15</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H63" s="8"/>
     </row>
@@ -3644,7 +3784,7 @@
         <v>15</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H64" s="8"/>
     </row>
@@ -3661,7 +3801,7 @@
         <v>15</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H65" s="8"/>
     </row>
@@ -3751,7 +3891,7 @@
         <v>15</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H70" s="8"/>
     </row>
@@ -3799,11 +3939,11 @@
         <v>1</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F73" s="11"/>
       <c r="G73" s="9"/>
@@ -3853,13 +3993,13 @@
         <v>3</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H76" s="8"/>
     </row>
@@ -3871,13 +4011,13 @@
         <v>4</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H77" s="8"/>
     </row>
@@ -3913,7 +4053,7 @@
         <v>15</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H79" s="8"/>
     </row>
@@ -3943,13 +4083,13 @@
         <v>8</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H81" s="8"/>
     </row>
@@ -3961,13 +4101,13 @@
         <v>9</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H82" s="8"/>
     </row>
@@ -3979,49 +4119,49 @@
         <v>10</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H83" s="8"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="2">
-        <v>11</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H84" s="8"/>
+      <c r="A84" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="6">
+        <v>2</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D84" s="11"/>
+      <c r="E84" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84" s="11"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
       <c r="D85" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="H85" s="8"/>
     </row>
@@ -4030,16 +4170,16 @@
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
       <c r="D86" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="H86" s="8"/>
     </row>
@@ -4047,50 +4187,90 @@
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="8"/>
+      <c r="D87" s="2">
+        <v>3</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="H87" s="8"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="8"/>
+      <c r="D88" s="2">
+        <v>4</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="H88" s="8"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
+      <c r="D89" s="2">
+        <v>5</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="H89" s="8"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="8"/>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8"/>
+      <c r="D90" s="2">
+        <v>6</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="H90" s="8"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
+      <c r="D91" s="2">
+        <v>7</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="H91" s="8"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
@@ -11602,36 +11782,6 @@
       <c r="F842" s="8"/>
       <c r="G842" s="8"/>
       <c r="H842" s="8"/>
-    </row>
-    <row r="843" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A843" s="8"/>
-      <c r="B843" s="8"/>
-      <c r="C843" s="8"/>
-      <c r="D843" s="2"/>
-      <c r="E843" s="8"/>
-      <c r="F843" s="8"/>
-      <c r="G843" s="8"/>
-      <c r="H843" s="8"/>
-    </row>
-    <row r="844" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A844" s="8"/>
-      <c r="B844" s="8"/>
-      <c r="C844" s="8"/>
-      <c r="D844" s="2"/>
-      <c r="E844" s="8"/>
-      <c r="F844" s="8"/>
-      <c r="G844" s="8"/>
-      <c r="H844" s="8"/>
-    </row>
-    <row r="845" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A845" s="8"/>
-      <c r="B845" s="8"/>
-      <c r="C845" s="8"/>
-      <c r="D845" s="2"/>
-      <c r="E845" s="8"/>
-      <c r="F845" s="8"/>
-      <c r="G845" s="8"/>
-      <c r="H845" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -11646,143 +11796,157 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="F38:F43 F45:F49 F67:F70 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65">
-    <cfRule type="expression" dxfId="47" priority="61">
+    <cfRule type="expression" dxfId="55" priority="77">
       <formula>$F9="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="62">
+    <cfRule type="expression" dxfId="54" priority="78">
       <formula>$F9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="63">
+    <cfRule type="expression" dxfId="53" priority="79">
       <formula>$F9="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="64">
+    <cfRule type="expression" dxfId="52" priority="80">
       <formula>$F9="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71">
-    <cfRule type="expression" dxfId="43" priority="49">
+    <cfRule type="expression" dxfId="51" priority="65">
       <formula>$F71="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="50">
+    <cfRule type="expression" dxfId="50" priority="66">
       <formula>$F71="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="51">
+    <cfRule type="expression" dxfId="49" priority="67">
       <formula>$F71="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="52">
+    <cfRule type="expression" dxfId="48" priority="68">
       <formula>$F71="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F72">
-    <cfRule type="expression" dxfId="39" priority="41">
+    <cfRule type="expression" dxfId="47" priority="57">
       <formula>$F72="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="42">
+    <cfRule type="expression" dxfId="46" priority="58">
       <formula>$F72="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="43">
+    <cfRule type="expression" dxfId="45" priority="59">
       <formula>$F72="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="44">
+    <cfRule type="expression" dxfId="44" priority="60">
       <formula>$F72="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F74:F77">
-    <cfRule type="expression" dxfId="35" priority="33">
+    <cfRule type="expression" dxfId="43" priority="49">
       <formula>$F74="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="34">
+    <cfRule type="expression" dxfId="42" priority="50">
       <formula>$F74="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="35">
+    <cfRule type="expression" dxfId="41" priority="51">
       <formula>$F74="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="36">
+    <cfRule type="expression" dxfId="40" priority="52">
       <formula>$F74="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F78">
-    <cfRule type="expression" dxfId="31" priority="29">
+    <cfRule type="expression" dxfId="39" priority="45">
       <formula>$F78="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="30">
+    <cfRule type="expression" dxfId="38" priority="46">
       <formula>$F78="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="31">
+    <cfRule type="expression" dxfId="37" priority="47">
       <formula>$F78="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="32">
+    <cfRule type="expression" dxfId="36" priority="48">
       <formula>$F78="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F79">
-    <cfRule type="expression" dxfId="27" priority="25">
+    <cfRule type="expression" dxfId="35" priority="41">
       <formula>$F79="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="26">
+    <cfRule type="expression" dxfId="34" priority="42">
       <formula>$F79="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="33" priority="43">
       <formula>$F79="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="28">
+    <cfRule type="expression" dxfId="32" priority="44">
       <formula>$F79="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86">
-    <cfRule type="expression" dxfId="15" priority="13">
-      <formula>$F86="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
-      <formula>$F86="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>$F86="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>$F86="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F80:F83">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>$F80="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="26" priority="26">
       <formula>$F80="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>$F80="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="24" priority="28">
       <formula>$F80="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F84">
+  <conditionalFormatting sqref="F85:F87">
+    <cfRule type="expression" dxfId="15" priority="13">
+      <formula>$F85="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="14">
+      <formula>$F85="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>$F85="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>$F85="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F88">
+    <cfRule type="expression" dxfId="11" priority="9">
+      <formula>$F88="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>$F88="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>$F88="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="12">
+      <formula>$F88="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F89:F90">
     <cfRule type="expression" dxfId="7" priority="5">
-      <formula>$F84="Open"</formula>
+      <formula>$F89="Open"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$F84="Passed"</formula>
+      <formula>$F89="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="7">
-      <formula>$F84="Failed"</formula>
+      <formula>$F89="Failed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="8">
-      <formula>$F84="In work"</formula>
+      <formula>$F89="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F85">
+  <conditionalFormatting sqref="F91">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$F85="Open"</formula>
+      <formula>$F91="Open"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$F85="Passed"</formula>
+      <formula>$F91="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$F85="Failed"</formula>
+      <formula>$F91="Failed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$F85="In work"</formula>
+      <formula>$F91="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -11797,7 +11961,7 @@
           <x14:formula1>
             <xm:f>'Possible results'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F38:F43 F45:F49 F67:F72 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65 F74:F86</xm:sqref>
+          <xm:sqref>F38:F43 F45:F49 F67:F72 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65 F74:F83 F85:F91</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11810,7 +11974,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11831,16 +11995,14 @@
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>90</v>
-      </c>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -11860,7 +12022,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Product page 3rd test case done
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71350A99-87EA-4473-9614-B8B84A554274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985A8879-68A7-4A3E-8685-B17C35984E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="133">
   <si>
     <t>Test plan</t>
   </si>
@@ -607,9 +607,6 @@
   </si>
   <si>
     <t>Open product and check actions which can be performed on product</t>
-  </si>
-  <si>
-    <t>To iste ale poslat request a na zaklade response skontrolovat ci su zobrazene na stranke dobre udaje</t>
   </si>
   <si>
     <t>Registracia testy</t>
@@ -836,6 +833,21 @@
   </si>
   <si>
     <t>Last size is not possible to add to cart</t>
+  </si>
+  <si>
+    <t>P-003 Product page with request info</t>
+  </si>
+  <si>
+    <t>Product page successfully opened</t>
+  </si>
+  <si>
+    <t>Send request to obtain product info</t>
+  </si>
+  <si>
+    <t>Response of the request contains correct info which is also displayed in the product page like: product title, response length is 1, status of the product is active, variant of the product is size and has length 3, sizes in the webpage are the same as from the response, url contains info from response</t>
+  </si>
+  <si>
+    <t>Open product and compare info from website with info from response</t>
   </si>
 </sst>
 </file>
@@ -963,7 +975,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1016,186 +1028,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <fill>
         <patternFill>
@@ -2552,8 +2399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
   <dimension ref="A1:V842"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2685,7 +2532,7 @@
       <c r="B5" s="19"/>
       <c r="C5" s="17">
         <f ca="1">TODAY()</f>
-        <v>45005</v>
+        <v>45006</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -2783,7 +2630,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>23</v>
@@ -2858,7 +2705,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>23</v>
@@ -2896,7 +2743,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>23</v>
@@ -2984,13 +2831,13 @@
         <v>3</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>23</v>
@@ -3009,7 +2856,7 @@
         <v>13</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>23</v>
@@ -3078,7 +2925,7 @@
         <v>13</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>23</v>
@@ -3371,7 +3218,7 @@
         <v>13</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>23</v>
@@ -3391,7 +3238,7 @@
         <v>13</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>23</v>
@@ -3411,7 +3258,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>23</v>
@@ -3503,7 +3350,7 @@
         <v>15</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H48" s="8"/>
     </row>
@@ -3521,7 +3368,7 @@
         <v>15</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H49" s="8"/>
     </row>
@@ -3537,7 +3384,7 @@
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F50" s="11"/>
       <c r="G50" s="9"/>
@@ -3593,7 +3440,7 @@
         <v>15</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H53" s="8"/>
     </row>
@@ -3605,13 +3452,13 @@
         <v>4</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H54" s="8"/>
     </row>
@@ -3623,13 +3470,13 @@
         <v>5</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H55" s="8"/>
     </row>
@@ -3647,7 +3494,7 @@
         <v>15</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H56" s="8"/>
     </row>
@@ -3716,7 +3563,7 @@
         <v>15</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H60" s="8"/>
     </row>
@@ -3727,13 +3574,13 @@
         <v>5</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H61" s="8"/>
     </row>
@@ -3767,7 +3614,7 @@
         <v>15</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H63" s="8"/>
     </row>
@@ -3784,7 +3631,7 @@
         <v>15</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H64" s="8"/>
     </row>
@@ -3801,7 +3648,7 @@
         <v>15</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H65" s="8"/>
     </row>
@@ -3891,7 +3738,7 @@
         <v>15</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H70" s="8"/>
     </row>
@@ -3939,7 +3786,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="9" t="s">
@@ -3993,13 +3840,13 @@
         <v>3</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H76" s="8"/>
     </row>
@@ -4011,13 +3858,13 @@
         <v>4</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H77" s="8"/>
     </row>
@@ -4053,7 +3900,7 @@
         <v>15</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H79" s="8"/>
     </row>
@@ -4083,13 +3930,13 @@
         <v>8</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H81" s="8"/>
     </row>
@@ -4101,13 +3948,13 @@
         <v>9</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H82" s="8"/>
     </row>
@@ -4119,13 +3966,13 @@
         <v>10</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H83" s="8"/>
     </row>
@@ -4137,7 +3984,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D84" s="11"/>
       <c r="E84" s="9" t="s">
@@ -4191,13 +4038,13 @@
         <v>3</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H87" s="8"/>
     </row>
@@ -4209,13 +4056,13 @@
         <v>4</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H88" s="8"/>
     </row>
@@ -4227,13 +4074,13 @@
         <v>5</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H89" s="8"/>
     </row>
@@ -4245,13 +4092,13 @@
         <v>6</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H90" s="8"/>
     </row>
@@ -4263,84 +4110,124 @@
         <v>7</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H91" s="8"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="8"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
+      <c r="A92" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B92" s="6">
+        <v>3</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D92" s="11"/>
+      <c r="E92" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F92" s="11"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
+      <c r="D93" s="2">
+        <v>1</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
+      <c r="D94" s="2">
+        <v>2</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H94" s="8"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
+      <c r="D95" s="2">
+        <v>3</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="H95" s="8"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
+      <c r="D96" s="22">
+        <v>4</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F96" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G96" s="20" t="s">
+        <v>131</v>
+      </c>
       <c r="H96" s="8"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="20"/>
       <c r="H97" s="8"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="20"/>
       <c r="H98" s="8"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
@@ -11784,7 +11671,11 @@
       <c r="H842" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="G96:G98"/>
+    <mergeCell ref="E96:E98"/>
+    <mergeCell ref="D96:D98"/>
+    <mergeCell ref="F96:F98"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="C3:V3"/>
     <mergeCell ref="A3:B3"/>
@@ -11796,157 +11687,171 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="F38:F43 F45:F49 F67:F70 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65">
-    <cfRule type="expression" dxfId="55" priority="77">
+    <cfRule type="expression" dxfId="47" priority="81">
       <formula>$F9="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="78">
+    <cfRule type="expression" dxfId="46" priority="82">
       <formula>$F9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="79">
+    <cfRule type="expression" dxfId="45" priority="83">
       <formula>$F9="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="80">
+    <cfRule type="expression" dxfId="44" priority="84">
       <formula>$F9="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71">
-    <cfRule type="expression" dxfId="51" priority="65">
+    <cfRule type="expression" dxfId="43" priority="69">
       <formula>$F71="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="66">
+    <cfRule type="expression" dxfId="42" priority="70">
       <formula>$F71="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="67">
+    <cfRule type="expression" dxfId="41" priority="71">
       <formula>$F71="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="68">
+    <cfRule type="expression" dxfId="40" priority="72">
       <formula>$F71="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F72">
-    <cfRule type="expression" dxfId="47" priority="57">
+    <cfRule type="expression" dxfId="39" priority="61">
       <formula>$F72="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="58">
+    <cfRule type="expression" dxfId="38" priority="62">
       <formula>$F72="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="59">
+    <cfRule type="expression" dxfId="37" priority="63">
       <formula>$F72="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="60">
+    <cfRule type="expression" dxfId="36" priority="64">
       <formula>$F72="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F74:F77">
-    <cfRule type="expression" dxfId="43" priority="49">
+    <cfRule type="expression" dxfId="35" priority="53">
       <formula>$F74="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="50">
+    <cfRule type="expression" dxfId="34" priority="54">
       <formula>$F74="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="51">
+    <cfRule type="expression" dxfId="33" priority="55">
       <formula>$F74="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="52">
+    <cfRule type="expression" dxfId="32" priority="56">
       <formula>$F74="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F78">
-    <cfRule type="expression" dxfId="39" priority="45">
+    <cfRule type="expression" dxfId="31" priority="49">
       <formula>$F78="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="46">
+    <cfRule type="expression" dxfId="30" priority="50">
       <formula>$F78="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="47">
+    <cfRule type="expression" dxfId="29" priority="51">
       <formula>$F78="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="48">
+    <cfRule type="expression" dxfId="28" priority="52">
       <formula>$F78="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F79">
-    <cfRule type="expression" dxfId="35" priority="41">
+    <cfRule type="expression" dxfId="27" priority="45">
       <formula>$F79="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="42">
+    <cfRule type="expression" dxfId="26" priority="46">
       <formula>$F79="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="43">
+    <cfRule type="expression" dxfId="25" priority="47">
       <formula>$F79="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="44">
+    <cfRule type="expression" dxfId="24" priority="48">
       <formula>$F79="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F80:F83">
-    <cfRule type="expression" dxfId="27" priority="25">
+    <cfRule type="expression" dxfId="23" priority="29">
       <formula>$F80="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="26">
+    <cfRule type="expression" dxfId="22" priority="30">
       <formula>$F80="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="21" priority="31">
       <formula>$F80="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="28">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>$F80="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F85:F87">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="19" priority="17">
       <formula>$F85="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="18" priority="18">
       <formula>$F85="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>$F85="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>$F85="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F88">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>$F88="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>$F88="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>$F88="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>$F88="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F89:F90">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>$F89="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>$F89="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>$F89="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>$F89="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F91">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>$F91="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>$F91="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>$F91="Failed"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>$F91="In work"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F93:F96">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$F93="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$F93="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$F93="Failed"</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$F91="In work"</formula>
+      <formula>$F93="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -11961,7 +11866,7 @@
           <x14:formula1>
             <xm:f>'Possible results'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F38:F43 F45:F49 F67:F72 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65 F74:F83 F85:F91</xm:sqref>
+          <xm:sqref>F38:F43 F45:F49 F67:F72 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65 F74:F83 F85:F91 F93:F95</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11973,8 +11878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC3EE7E-7188-42AF-B965-808431552D03}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12001,9 +11906,7 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="C4" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" s="8" t="s">
@@ -12022,7 +11925,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
product page test case 4 done
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985A8879-68A7-4A3E-8685-B17C35984E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F25908-7382-47BD-BD3D-7028CB907A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
+    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="143">
   <si>
     <t>Test plan</t>
   </si>
@@ -848,6 +848,36 @@
   </si>
   <si>
     <t>Open product and compare info from website with info from response</t>
+  </si>
+  <si>
+    <t>P-004 Cart sidebar actions</t>
+  </si>
+  <si>
+    <t>Open product, add it to cart and check cart sidebar</t>
+  </si>
+  <si>
+    <t>Click on Add to cart to add product to cart</t>
+  </si>
+  <si>
+    <t>Sidebar cart is opened, product name, subtotal and total prices, shipping info, quantity info are correct and decrease button is disabled</t>
+  </si>
+  <si>
+    <t>Increase product quantity</t>
+  </si>
+  <si>
+    <t>Quantity has been increased (2 products in cart)</t>
+  </si>
+  <si>
+    <t>Remove product from cart</t>
+  </si>
+  <si>
+    <t>Product successfully removed from cart and cart is empty</t>
+  </si>
+  <si>
+    <t>Close sidebar cart</t>
+  </si>
+  <si>
+    <t>Sidebar cart is closed and page with product is visible</t>
   </si>
 </sst>
 </file>
@@ -975,7 +1005,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1007,6 +1037,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1029,20 +1068,14 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -1479,27 +1512,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -1569,507 +1581,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -2399,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
   <dimension ref="A1:V842"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="C83" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2416,143 +1927,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="17">
+      <c r="B5" s="22"/>
+      <c r="C5" s="20">
         <f ca="1">TODAY()</f>
-        <v>45006</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
+        <v>45007</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
     </row>
     <row r="7" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -4196,16 +3707,16 @@
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="22">
+      <c r="D96" s="15">
         <v>4</v>
       </c>
-      <c r="E96" s="21" t="s">
+      <c r="E96" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="F96" s="22" t="s">
+      <c r="F96" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G96" s="20" t="s">
+      <c r="G96" s="13" t="s">
         <v>131</v>
       </c>
       <c r="H96" s="8"/>
@@ -4214,110 +3725,174 @@
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="22"/>
-      <c r="E97" s="21"/>
-      <c r="F97" s="22"/>
-      <c r="G97" s="20"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="13"/>
       <c r="H97" s="8"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="22"/>
-      <c r="E98" s="21"/>
-      <c r="F98" s="22"/>
-      <c r="G98" s="20"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="13"/>
       <c r="H98" s="8"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" s="8"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="8"/>
-      <c r="H99" s="8"/>
+      <c r="A99" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B99" s="6">
+        <v>4</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D99" s="11"/>
+      <c r="E99" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F99" s="11"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="8"/>
+      <c r="D100" s="2">
+        <v>1</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G100" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H100" s="8"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="8"/>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="8"/>
+      <c r="D101" s="2">
+        <v>2</v>
+      </c>
+      <c r="E101" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H101" s="8"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="8"/>
+      <c r="D102" s="2">
+        <v>3</v>
+      </c>
+      <c r="E102" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G102" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="H102" s="8"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="8"/>
+      <c r="D103" s="15">
+        <v>4</v>
+      </c>
+      <c r="E103" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F103" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G103" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="H103" s="8"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="8"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="14"/>
       <c r="H104" s="8"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="8"/>
-      <c r="G105" s="8"/>
+      <c r="D105" s="2">
+        <v>5</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="H105" s="8"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="8"/>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="8"/>
-      <c r="G106" s="8"/>
+      <c r="D106" s="2">
+        <v>6</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="H106" s="8"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="8"/>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8"/>
-      <c r="G107" s="8"/>
+      <c r="D107" s="2">
+        <v>7</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G107" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="H107" s="8"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
@@ -11671,7 +11246,11 @@
       <c r="H842" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="17">
+    <mergeCell ref="G103:G104"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="D103:D104"/>
     <mergeCell ref="G96:G98"/>
     <mergeCell ref="E96:E98"/>
     <mergeCell ref="D96:D98"/>
@@ -11686,172 +11265,88 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F38:F43 F45:F49 F67:F70 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65">
-    <cfRule type="expression" dxfId="47" priority="81">
+  <conditionalFormatting sqref="F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F38:F43 F45:F49 F51:F56 F58:F65">
+    <cfRule type="expression" dxfId="23" priority="96">
+      <formula>$F9="In work"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="93">
       <formula>$F9="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="82">
+    <cfRule type="expression" dxfId="21" priority="94">
       <formula>$F9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="83">
+    <cfRule type="expression" dxfId="20" priority="95">
       <formula>$F9="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="84">
-      <formula>$F9="In work"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F67:F72">
+    <cfRule type="expression" dxfId="19" priority="73">
+      <formula>$F67="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="74">
+      <formula>$F67="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="75">
+      <formula>$F67="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="76">
+      <formula>$F67="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F71">
-    <cfRule type="expression" dxfId="43" priority="69">
-      <formula>$F71="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="70">
-      <formula>$F71="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="71">
-      <formula>$F71="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="72">
-      <formula>$F71="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F72">
-    <cfRule type="expression" dxfId="39" priority="61">
-      <formula>$F72="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="62">
-      <formula>$F72="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="63">
-      <formula>$F72="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="64">
-      <formula>$F72="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F74:F77">
-    <cfRule type="expression" dxfId="35" priority="53">
+  <conditionalFormatting sqref="F74:F96">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>$F74="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="54">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>$F74="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="55">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>$F74="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="56">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>$F74="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F78">
-    <cfRule type="expression" dxfId="31" priority="49">
-      <formula>$F78="Open"</formula>
+  <conditionalFormatting sqref="F99">
+    <cfRule type="expression" dxfId="11" priority="9">
+      <formula>$F99="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="50">
-      <formula>$F78="Passed"</formula>
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>$F99="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="51">
-      <formula>$F78="Failed"</formula>
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>$F99="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="52">
-      <formula>$F78="In work"</formula>
+    <cfRule type="expression" dxfId="8" priority="12">
+      <formula>$F99="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F79">
-    <cfRule type="expression" dxfId="27" priority="45">
-      <formula>$F79="Open"</formula>
+  <conditionalFormatting sqref="F100:F103">
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>$F100="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="46">
-      <formula>$F79="Passed"</formula>
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>$F100="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="47">
-      <formula>$F79="Failed"</formula>
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>$F100="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="48">
-      <formula>$F79="In work"</formula>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>$F100="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F80:F83">
-    <cfRule type="expression" dxfId="23" priority="29">
-      <formula>$F80="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="30">
-      <formula>$F80="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="31">
-      <formula>$F80="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="32">
-      <formula>$F80="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F85:F87">
-    <cfRule type="expression" dxfId="19" priority="17">
-      <formula>$F85="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
-      <formula>$F85="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="19">
-      <formula>$F85="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
-      <formula>$F85="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F88">
-    <cfRule type="expression" dxfId="15" priority="13">
-      <formula>$F88="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
-      <formula>$F88="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>$F88="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>$F88="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F89:F90">
-    <cfRule type="expression" dxfId="11" priority="9">
-      <formula>$F89="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>$F89="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>$F89="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
-      <formula>$F89="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F91">
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>$F91="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$F91="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>$F91="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>$F91="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F93:F96">
+  <conditionalFormatting sqref="F105:F107">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$F93="Open"</formula>
+      <formula>$F105="Open"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$F93="Passed"</formula>
+      <formula>$F105="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$F93="Failed"</formula>
+      <formula>$F105="Failed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$F93="In work"</formula>
+      <formula>$F105="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -11861,12 +11356,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56147D66-2DCC-4DA7-ACD5-C3DA6B36A0CA}">
           <x14:formula1>
             <xm:f>'Possible results'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F38:F43 F45:F49 F67:F72 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65 F74:F83 F85:F91 F93:F95</xm:sqref>
+          <xm:sqref>F38:F43 F45:F49 F67:F72 F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F51:F56 F58:F65 F74:F83 F85:F91 F93:F95 F100:F102 F105:F107</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11878,8 +11373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC3EE7E-7188-42AF-B965-808431552D03}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add to cart and checkout E2E test case done
</commit_message>
<xml_diff>
--- a/CypressTestingTestCases.xlsx
+++ b/CypressTestingTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boros\Desktop\Cypress testing My\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F25908-7382-47BD-BD3D-7028CB907A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC0E8C9-CD51-4C4A-B5C5-C679DE9F8C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9BCE072E-4C94-4026-A086-55E49C5F1C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="145">
   <si>
     <t>Test plan</t>
   </si>
@@ -878,6 +878,12 @@
   </si>
   <si>
     <t>Sidebar cart is closed and page with product is visible</t>
+  </si>
+  <si>
+    <t>Open product, add it to cart and proceed to checkout</t>
+  </si>
+  <si>
+    <t>P-005 E2E Add a product to the cart and checkout</t>
   </si>
 </sst>
 </file>
@@ -1038,13 +1044,16 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1067,15 +1076,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -1424,180 +1430,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1910,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320106A2-112A-4206-867D-24B4C435AD62}">
   <dimension ref="A1:V842"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C83" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103:E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1927,143 +1759,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="20">
+      <c r="B5" s="23"/>
+      <c r="C5" s="21">
         <f ca="1">TODAY()</f>
         <v>45007</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
     </row>
     <row r="7" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -3707,16 +3539,16 @@
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="15">
+      <c r="D96" s="14">
         <v>4</v>
       </c>
-      <c r="E96" s="14" t="s">
+      <c r="E96" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="F96" s="15" t="s">
+      <c r="F96" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G96" s="13" t="s">
+      <c r="G96" s="16" t="s">
         <v>131</v>
       </c>
       <c r="H96" s="8"/>
@@ -3725,20 +3557,20 @@
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="15"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="13"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="16"/>
       <c r="H97" s="8"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="15"/>
-      <c r="G98" s="13"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="16"/>
       <c r="H98" s="8"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
@@ -3817,16 +3649,16 @@
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
-      <c r="D103" s="15">
+      <c r="D103" s="14">
         <v>4</v>
       </c>
-      <c r="E103" s="23" t="s">
+      <c r="E103" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="F103" s="15" t="s">
+      <c r="F103" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G103" s="14" t="s">
+      <c r="G103" s="13" t="s">
         <v>136</v>
       </c>
       <c r="H103" s="8"/>
@@ -3835,10 +3667,10 @@
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="23"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="13"/>
       <c r="H104" s="8"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
@@ -3896,14 +3728,22 @@
       <c r="H107" s="8"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A108" s="8"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
+      <c r="A108" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B108" s="6">
+        <v>5</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D108" s="11"/>
+      <c r="E108" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F108" s="11"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="8"/>
@@ -11247,14 +11087,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G103:G104"/>
-    <mergeCell ref="F103:F104"/>
-    <mergeCell ref="E103:E104"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="G96:G98"/>
-    <mergeCell ref="E96:E98"/>
-    <mergeCell ref="D96:D98"/>
-    <mergeCell ref="F96:F98"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="C3:V3"/>
     <mergeCell ref="A3:B3"/>
@@ -11264,89 +11096,69 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G103:G104"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="G96:G98"/>
+    <mergeCell ref="E96:E98"/>
+    <mergeCell ref="D96:D98"/>
+    <mergeCell ref="F96:F98"/>
   </mergeCells>
   <conditionalFormatting sqref="F9:F11 F13:F17 F19:F22 F24:F27 F29:F36 F38:F43 F45:F49 F51:F56 F58:F65">
-    <cfRule type="expression" dxfId="23" priority="96">
-      <formula>$F9="In work"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="93">
+    <cfRule type="expression" dxfId="15" priority="93">
       <formula>$F9="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="94">
+    <cfRule type="expression" dxfId="14" priority="94">
       <formula>$F9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="95">
+    <cfRule type="expression" dxfId="13" priority="95">
       <formula>$F9="Failed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="96">
+      <formula>$F9="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F67:F72">
-    <cfRule type="expression" dxfId="19" priority="73">
+    <cfRule type="expression" dxfId="11" priority="73">
       <formula>$F67="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="74">
+    <cfRule type="expression" dxfId="10" priority="74">
       <formula>$F67="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="75">
+    <cfRule type="expression" dxfId="9" priority="75">
       <formula>$F67="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="76">
+    <cfRule type="expression" dxfId="8" priority="76">
       <formula>$F67="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F74:F96">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>$F74="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>$F74="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="5" priority="15">
       <formula>$F74="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="4" priority="16">
       <formula>$F74="In work"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F99">
-    <cfRule type="expression" dxfId="11" priority="9">
+  <conditionalFormatting sqref="F99:F108">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F99="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$F99="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$F99="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$F99="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F100:F103">
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>$F100="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$F100="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>$F100="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>$F100="In work"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F105:F107">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$F105="Open"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$F105="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$F105="Failed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$F105="In work"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>